<commit_message>
Added new data visualization for sector of activity
</commit_message>
<xml_diff>
--- a/data/ateco_nace_table.xlsx
+++ b/data/ateco_nace_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/francesco_funghi_ulb_be/Documents/Desktop/Thesis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitelibrebruxelles-my.sharepoint.com/personal/francesco_funghi_ulb_be/Documents/Desktop/confiscated_companies/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_2CE8F5AA20D13884E901A5E0FB70EDEC1EA77266" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B789C5C1-423D-4292-B5A9-09514D957C58}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_2CE8F5AA20D13884E901A5E0FB70EDEC1EA77266" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55DE4B29-25F3-496B-9DF0-99EA401FAC1B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18444,10 +18444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3158"/>
+  <dimension ref="A1:S3158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
@@ -18455,9 +18455,13 @@
     <col min="1" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="66.21875" customWidth="1"/>
     <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="86.6640625" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" customWidth="1"/>
+    <col min="19" max="19" width="76.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6023</v>
       </c>
@@ -18470,8 +18474,9 @@
       <c r="D1" s="1" t="s">
         <v>6024</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3137</v>
       </c>
@@ -18485,7 +18490,7 @@
         <v>3157</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -18499,7 +18504,7 @@
         <v>3158</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -18513,7 +18518,7 @@
         <v>3159</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -18527,7 +18532,7 @@
         <v>3160</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -18541,7 +18546,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -18555,7 +18560,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -18569,7 +18574,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -18583,7 +18588,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -18597,7 +18602,7 @@
         <v>3163</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -18611,7 +18616,7 @@
         <v>3163</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -18625,7 +18630,7 @@
         <v>3164</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -18639,7 +18644,7 @@
         <v>3164</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -18653,7 +18658,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -18667,7 +18672,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -62585,7 +62590,7 @@
         <v>5174</v>
       </c>
     </row>
-    <row r="3153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3153" t="s">
         <v>3156</v>
       </c>
@@ -62599,7 +62604,7 @@
         <v>5175</v>
       </c>
     </row>
-    <row r="3154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3154" t="s">
         <v>3132</v>
       </c>
@@ -62613,7 +62618,7 @@
         <v>5175</v>
       </c>
     </row>
-    <row r="3155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3155" t="s">
         <v>3133</v>
       </c>
@@ -62627,7 +62632,7 @@
         <v>5175</v>
       </c>
     </row>
-    <row r="3156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3156" t="s">
         <v>3134</v>
       </c>
@@ -62641,7 +62646,7 @@
         <v>5176</v>
       </c>
     </row>
-    <row r="3157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3157" t="s">
         <v>3135</v>
       </c>
@@ -62655,7 +62660,7 @@
         <v>5176</v>
       </c>
     </row>
-    <row r="3158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3158" s="2" t="s">
         <v>3136</v>
       </c>
@@ -62668,11 +62673,11 @@
       <c r="D3158" s="2" t="s">
         <v>5176</v>
       </c>
+      <c r="E3158" s="2"/>
+      <c r="R3158" s="2"/>
+      <c r="S3158" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H3158">
-    <sortCondition ref="B2:B3158"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;A</oddHeader>

</xml_diff>